<commit_message>
commit modify db_outline/ rename dollars to funds
</commit_message>
<xml_diff>
--- a/Layout/DatabaseOutline.xlsx
+++ b/Layout/DatabaseOutline.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Table Name</t>
   </si>
@@ -21,7 +21,7 @@
     <t>user_table</t>
   </si>
   <si>
-    <t xml:space="preserve">userID AUTOINCREMENT INTEGER PRIMARY</t>
+    <t xml:space="preserve">Id AUTOINCREMENT INTEGER PRIMARY</t>
   </si>
   <si>
     <t xml:space="preserve">userName TEXT</t>
@@ -30,13 +30,13 @@
     <t xml:space="preserve"> password TEXT</t>
   </si>
   <si>
-    <t xml:space="preserve">allocatedFunds DOUBLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unallocatedFunds DOUBLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isLoggedIn TEXT</t>
+    <t xml:space="preserve">email TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt DATETIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unallocatedDollars DOUBLE</t>
   </si>
   <si>
     <t>"stanzu10"</t>
@@ -45,7 +45,10 @@
     <t>"password"</t>
   </si>
   <si>
-    <t>"True"</t>
+    <t>"bbastanza@something.com"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 19 Nov 2020 12:23:38 PM PST</t>
   </si>
   <si>
     <t>"sammy_shortcakes"</t>
@@ -54,19 +57,25 @@
     <t>"passing32"</t>
   </si>
   <si>
+    <t>"samcakes@confetti.com"</t>
+  </si>
+  <si>
     <t>"joey-bagOdoughnuts"</t>
   </si>
   <si>
     <t>"dunkin"</t>
   </si>
   <si>
-    <t>"False"</t>
+    <t>"joey@baggs.org"</t>
   </si>
   <si>
     <t>holding_table</t>
   </si>
   <si>
-    <t xml:space="preserve">id INTERGER PRIMARY</t>
+    <t xml:space="preserve">Id AUTOINCREMENT INTERGER PRIMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userId INT</t>
   </si>
   <si>
     <t xml:space="preserve">symbol TEXT</t>
@@ -75,9 +84,6 @@
     <t xml:space="preserve">companyName TEXT</t>
   </si>
   <si>
-    <t xml:space="preserve">value DOUBLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">totalShares DOUBLE</t>
   </si>
   <si>
@@ -103,16 +109,46 @@
   </si>
   <si>
     <t>"Amazon"</t>
+  </si>
+  <si>
+    <t>transaction_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holdingId INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sharesAmount DOUBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purchasePrice DOUBLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -138,17 +174,54 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color theme="1" tint="0"/>
+      <b/>
+      <color theme="0" tint="0"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF006100"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C0006"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
       <sz val="14"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -162,30 +235,6 @@
         <bgColor theme="1" tint="0.34998626667073579"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor theme="4" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor theme="8" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor theme="7" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -211,10 +260,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thin">
         <color theme="1"/>
       </left>
-      <right style="hair">
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
@@ -250,9 +299,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color theme="1"/>
       </right>
@@ -265,24 +312,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="3" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="3" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="4" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="4" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="7" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="4" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="6" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="6" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="7" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="7" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="8" fillId="2" borderId="2" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="9" fillId="3" borderId="2" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="10" fillId="4" borderId="2" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="6" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,13 +848,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.421875"/>
-    <col customWidth="1" min="2" max="2" width="14.8515625"/>
-    <col customWidth="1" min="3" max="3" width="27.57421875"/>
-    <col customWidth="1" min="4" max="4" width="46.7109375"/>
-    <col customWidth="1" min="5" max="5" width="28.28125"/>
-    <col customWidth="1" min="6" max="6" width="31.140625"/>
-    <col customWidth="1" min="7" max="7" width="20.00390625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="21.421875"/>
+    <col customWidth="1" min="2" max="2" width="24.7109375"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="27.57421875"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="46.7109375"/>
+    <col customWidth="1" min="5" max="5" width="36.140625"/>
+    <col customWidth="1" min="6" max="6" width="37.8515625"/>
+    <col customWidth="1" min="7" max="7" width="31.57421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75">
@@ -834,74 +889,74 @@
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="18.75">
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6">
-        <v>1453.4300000000001</v>
-      </c>
-      <c r="F4" s="6">
-        <v>80950.320000000007</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="8">
+        <v>83221.960000000006</v>
+      </c>
     </row>
     <row r="5" ht="18.75">
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7">
-        <v>19782.380000000001</v>
-      </c>
-      <c r="F5" s="7">
-        <v>76898.779999999999</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>10</v>
+      <c r="G5" s="9">
+        <v>53827.449999999997</v>
       </c>
     </row>
     <row r="6" ht="18.75">
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="9">
-        <v>12987.629999999999</v>
-      </c>
-      <c r="F6" s="9">
-        <v>12343.9</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10">
+        <v>12987.309999999999</v>
       </c>
     </row>
     <row r="7" ht="18.75">
@@ -914,167 +969,294 @@
     </row>
     <row r="8" ht="18.75">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="E8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" ht="18.75">
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6">
-        <v>4357.9700000000003</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8">
         <v>11.779999999999999</v>
       </c>
-      <c r="G9" s="2"/>
     </row>
     <row r="10" ht="18.75">
-      <c r="B10" s="6">
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8">
+        <v>19.219999999999999</v>
+      </c>
+    </row>
+    <row r="11" ht="18.75">
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="6">
-        <v>3412.54</v>
-      </c>
-      <c r="F10" s="6">
-        <v>19.219999999999999</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" ht="18.75">
-      <c r="B11" s="6">
+      <c r="F11" s="9">
+        <v>8.5299999999999994</v>
+      </c>
+    </row>
+    <row r="12" ht="18.75">
+      <c r="B12" s="8">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="6">
-        <v>34987.209999999999</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="D12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="8">
         <v>2543.1900000000001</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" ht="18.75">
-      <c r="B12" s="10">
-        <v>2</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="10">
-        <v>3452.6700000000001</v>
-      </c>
-      <c r="F12" s="10">
-        <v>8.5299999999999994</v>
-      </c>
-      <c r="G12" s="2"/>
     </row>
     <row r="13" ht="18.75">
       <c r="B13" s="10">
-        <v>2</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="C13" s="10">
+        <v>3</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="10">
-        <v>89372.710000000006</v>
+        <v>26</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F13" s="10">
-        <v>4573.8900000000003</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>6.2199999999999998</v>
+      </c>
     </row>
     <row r="14" ht="18.75">
       <c r="B14" s="9">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="9">
+        <v>4573.8900000000003</v>
+      </c>
+    </row>
+    <row r="15" ht="18.75">
+      <c r="B15" s="10">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10">
         <v>3</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1212.54</v>
-      </c>
-      <c r="F14" s="9">
-        <v>6.2199999999999998</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" ht="18.75">
-      <c r="B15" s="9">
-        <v>3</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="9">
-        <v>3272.71</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="D15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10">
         <v>373.88999999999999</v>
       </c>
-      <c r="G15" s="2"/>
     </row>
     <row r="16" ht="18.75">
-      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="20" ht="14.25"/>
-    <row r="21" ht="14.25"/>
-    <row r="22" ht="14.25"/>
-    <row r="23" ht="14.25"/>
-    <row r="24" ht="14.25"/>
+    <row r="17" ht="18.75">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75">
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>12.73</v>
+      </c>
+      <c r="F18" s="8">
+        <v>332.22000000000003</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75">
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>3</v>
+      </c>
+      <c r="E19" s="9">
+        <v>37.32</v>
+      </c>
+      <c r="F19" s="9">
+        <v>222.43000000000001</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75">
+      <c r="B20" s="8">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>25.890000000000001</v>
+      </c>
+      <c r="F20" s="8">
+        <v>97.640000000000001</v>
+      </c>
+    </row>
+    <row r="21" ht="18.75">
+      <c r="B21" s="10">
+        <v>4</v>
+      </c>
+      <c r="C21" s="10">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10">
+        <v>5</v>
+      </c>
+      <c r="E21" s="10">
+        <v>213.97</v>
+      </c>
+      <c r="F21" s="10">
+        <v>13.449999999999999</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75">
+      <c r="B22" s="9">
+        <v>5</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9">
+        <v>6</v>
+      </c>
+      <c r="E22" s="9">
+        <v>135.87</v>
+      </c>
+      <c r="F22" s="9">
+        <v>621.10000000000002</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75">
+      <c r="B23" s="8">
+        <v>6</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4</v>
+      </c>
+      <c r="E23" s="8">
+        <v>21.629999999999999</v>
+      </c>
+      <c r="F23" s="8">
+        <v>105.67</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75">
+      <c r="B24" s="10">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
+        <v>7</v>
+      </c>
+      <c r="E24" s="10">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F24" s="10">
+        <v>32.780000000000001</v>
+      </c>
+    </row>
     <row r="25" ht="14.25"/>
     <row r="26" ht="14.25"/>
+    <row r="29" ht="18.75">
+      <c r="B29" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>